<commit_message>
・ApplicationResources.properties修正 ・Check_Admin.java修正 ・validation.xml修正 ・admin.jsp修正 ・試験仕様書（単体テスト）.xlsx作成
</commit_message>
<xml_diff>
--- a/Document/作業一覧ざっくり.xlsx
+++ b/Document/作業一覧ざっくり.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>開発準備</t>
     <rPh sb="0" eb="2">
@@ -850,7 +850,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1031,7 +1031,9 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>